<commit_message>
Framework creation in Progress
</commit_message>
<xml_diff>
--- a/TestCaseDriverSheet.xlsx
+++ b/TestCaseDriverSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Frameworks/GitHub_ProjectAutomatedTests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48419373-CA7B-CA42-95F5-4ACE9E93FDF5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A886DF-6EA2-4144-B6A7-9C7E9AAED1E3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27880" windowHeight="10180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27820" windowHeight="10180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseInfo" sheetId="2" r:id="rId1"/>
@@ -110,12 +110,6 @@
     <t>Test6</t>
   </si>
   <si>
-    <t>ignoretestfeatureA2</t>
-  </si>
-  <si>
-    <t>testfeatureA1</t>
-  </si>
-  <si>
     <t>com.api.tests.module1.Module1Test</t>
   </si>
   <si>
@@ -231,6 +225,12 @@
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>Test8</t>
+  </si>
+  <si>
+    <t>ignore</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -590,22 +590,22 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" t="s">
-        <v>40</v>
-      </c>
       <c r="K1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -616,25 +616,25 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" t="s">
         <v>47</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -642,22 +642,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
       <c r="J3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -665,25 +665,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -691,10 +691,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -706,7 +706,7 @@
         <v>9</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -714,10 +714,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -729,7 +729,7 @@
         <v>9</v>
       </c>
       <c r="J6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -737,22 +737,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
       <c r="J7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -760,57 +760,57 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -823,7 +823,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -857,10 +857,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -874,7 +874,7 @@
         <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -882,47 +882,47 @@
         <v>0</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K5" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K6" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K8" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K9" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K10" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K12" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -957,13 +957,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -971,7 +971,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>